<commit_message>
Updated all outlet pages generation engine
All pages have been updated to generate from their own set of menu workbooks
</commit_message>
<xml_diff>
--- a/files/menus/green_mountain/breakfast_greenmountain.xlsx
+++ b/files/menus/green_mountain/breakfast_greenmountain.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ollip\Documents\!!ProjectFiles\ajaxproto\files\menus\mtbenson_market\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ollip\Documents\!!ProjectFiles\ezrab_feedbc\files\menus\green_mountain\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4685F3AC-2ED5-4F7A-90B0-7F5DDF76D718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA3FB2F-3100-4900-944C-36C7613809C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6855" windowWidth="29040" windowHeight="15840" xr2:uid="{F9466112-CF85-4C07-B090-DE232439FD19}"/>
+    <workbookView xWindow="8475" yWindow="6840" windowWidth="24825" windowHeight="14220" xr2:uid="{F9466112-CF85-4C07-B090-DE232439FD19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>